<commit_message>
Dich city_selection_screen.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43F358-713D-4DD7-A5E9-1B6FED052FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698351FA-39A1-4673-A344-5C0D0E474213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -115,6 +115,54 @@
   </si>
   <si>
     <t>Không có dữ liệu ảnh để hiển thị.</t>
+  </si>
+  <si>
+    <t>No photos to display.</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Trước</t>
+  </si>
+  <si>
+    <t>Sau</t>
+  </si>
+  <si>
+    <t>Lưu tất cả</t>
+  </si>
+  <si>
+    <t>Save all</t>
+  </si>
+  <si>
+    <t>city_selection_screen.dart</t>
+  </si>
+  <si>
+    <t>Chọn vị trí</t>
+  </si>
+  <si>
+    <t>Select location</t>
+  </si>
+  <si>
+    <t>Auto-detect</t>
+  </si>
+  <si>
+    <t>Manually</t>
+  </si>
+  <si>
+    <t>Chọn thủ công</t>
+  </si>
+  <si>
+    <t>Tự động phát hiện</t>
+  </si>
+  <si>
+    <t>Search city/location…</t>
+  </si>
+  <si>
+    <t>Tìm kiếm địa danh…</t>
   </si>
 </sst>
 </file>
@@ -190,12 +238,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -478,19 +526,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -581,13 +629,13 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -606,32 +654,106 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dich edit_profile_screen.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698351FA-39A1-4673-A344-5C0D0E474213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC6FD6-B4EE-4DE9-ADCC-00FE203DC88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -163,6 +163,81 @@
   </si>
   <si>
     <t>Tìm kiếm địa danh…</t>
+  </si>
+  <si>
+    <t>edit_profile_screen.dart</t>
+  </si>
+  <si>
+    <t>Nam', 'Nữ', 'Khác'</t>
+  </si>
+  <si>
+    <t>Male', 'Female', 'Other'</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin</t>
+  </si>
+  <si>
+    <t>Edit profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic info </t>
+  </si>
+  <si>
+    <t>Thông tin cơ bản</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Not selected</t>
+  </si>
+  <si>
+    <t>Chưa có thông tin</t>
+  </si>
+  <si>
+    <t>Cân nặng</t>
+  </si>
+  <si>
+    <t>Chiều cao</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Interests &amp; Style</t>
+  </si>
+  <si>
+    <t>Sở thích &amp; Phong cách</t>
+  </si>
+  <si>
+    <t>Màu sắc yêu thích</t>
+  </si>
+  <si>
+    <t>Phong cách cá nhân</t>
+  </si>
+  <si>
+    <t>Personal style</t>
+  </si>
+  <si>
+    <t>Favorite colours</t>
   </si>
 </sst>
 </file>
@@ -232,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -244,6 +319,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -526,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,13 +826,125 @@
         <v>45</v>
       </c>
     </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dich outfit_detail_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC6FD6-B4EE-4DE9-ADCC-00FE203DC88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A48054-51C0-45A1-B7B5-4CE553072F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -234,10 +234,52 @@
     <t>Phong cách cá nhân</t>
   </si>
   <si>
+    <t>Favorite colors</t>
+  </si>
+  <si>
     <t>Personal style</t>
   </si>
   <si>
-    <t>Favorite colours</t>
+    <t>main_screen.dart</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Closets</t>
+  </si>
+  <si>
+    <t>Outfits</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Trang chủ</t>
+  </si>
+  <si>
+    <t>Tủ đồ</t>
+  </si>
+  <si>
+    <t>Trang phục</t>
+  </si>
+  <si>
+    <t>Cá nhân</t>
+  </si>
+  <si>
+    <t>outfit_detail_page.dart</t>
+  </si>
+  <si>
+    <t>Fixed outfit</t>
+  </si>
+  <si>
+    <t>Trang phục cố định</t>
+  </si>
+  <si>
+    <t>Các món đồ trong trang phục này luôn được mặc cùng nhau. Mỗi món đồ chỉ được thuộc một trang phục cố định</t>
+  </si>
+  <si>
+    <t>Items in this outfit are always worn together. Each item can only belong to one fixed outfit.</t>
   </si>
 </sst>
 </file>
@@ -604,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +964,7 @@
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>68</v>
@@ -930,14 +972,76 @@
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A53:B53"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>

</xml_diff>

<commit_message>
Dich settings_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A48054-51C0-45A1-B7B5-4CE553072F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5322A844-F27C-4B99-8FE3-C129D3342EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>Items in this outfit are always worn together. Each item can only belong to one fixed outfit.</t>
+  </si>
+  <si>
+    <t>settings_page.dart</t>
+  </si>
+  <si>
+    <t>Chọn ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Select language</t>
+  </si>
+  <si>
+    <t>Cài đặt</t>
   </si>
 </sst>
 </file>
@@ -646,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,10 +1050,51 @@
         <v>83</v>
       </c>
     </row>
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>

</xml_diff>

<commit_message>
Dich splash_screen.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5322A844-F27C-4B99-8FE3-C129D3342EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B6513-404F-4DAE-A81B-4AB91AA3C9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -292,6 +292,30 @@
   </si>
   <si>
     <t>Cài đặt</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Vị trí</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Cleaning closet…</t>
+  </si>
+  <si>
+    <t>Đang lau chùi tủ đồ</t>
+  </si>
+  <si>
+    <t>splash_screen.dart</t>
   </si>
 </sst>
 </file>
@@ -658,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,28 +1097,57 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+      <c r="A60" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="B60" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>

</xml_diff>

<commit_message>
Dich closet_detail_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B6513-404F-4DAE-A81B-4AB91AA3C9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC2875F-BE8F-4085-9D46-0E1988D40DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -316,6 +316,27 @@
   </si>
   <si>
     <t>splash_screen.dart</t>
+  </si>
+  <si>
+    <t>My first closet</t>
+  </si>
+  <si>
+    <t>Tủ đồ đầu tiên của tôi</t>
+  </si>
+  <si>
+    <t>closet_detail_page.dart</t>
+  </si>
+  <si>
+    <t>Lỗi:</t>
+  </si>
+  <si>
+    <t>Error:</t>
+  </si>
+  <si>
+    <t>Your closet is empty. Please add items!</t>
+  </si>
+  <si>
+    <t>Tủ của bạn đang trống. Hãy thêm đồ vật vào trước nhé!</t>
   </si>
 </sst>
 </file>
@@ -682,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,19 +1156,70 @@
       <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>

</xml_diff>

<commit_message>
Dich closets_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC2875F-BE8F-4085-9D46-0E1988D40DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA5FC87-86E6-4D89-B479-46088D6ACB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -336,7 +336,22 @@
     <t>Your closet is empty. Please add items!</t>
   </si>
   <si>
-    <t>Tủ của bạn đang trống. Hãy thêm đồ vật vào trước nhé!</t>
+    <t>closets_page.dart</t>
+  </si>
+  <si>
+    <t>Tạo tủ đồ mới</t>
+  </si>
+  <si>
+    <t>Tủ đồ của bạn đang trống. Hãy thêm đồ vật trước nhé!</t>
+  </si>
+  <si>
+    <t>Create new closet</t>
+  </si>
+  <si>
+    <t>Closet name</t>
+  </si>
+  <si>
+    <t>Tên tủ đồ</t>
   </si>
 </sst>
 </file>
@@ -406,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -421,6 +436,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -703,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,31 +1208,62 @@
         <v>102</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A73:B73"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A57:B57"/>

</xml_diff>

<commit_message>
Dich home_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA5FC87-86E6-4D89-B479-46088D6ACB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6417E61D-FD23-4A1D-8FE9-2811E9B8A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7485" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="140">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Are you sure to permanently delete item "A"?</t>
   </si>
   <si>
-    <t>Bạn có chắc chắn muốn xóa vĩnh viễn món đồ “…” không?</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -69,15 +66,9 @@
     <t>Edit item</t>
   </si>
   <si>
-    <t>Sửa món đồ</t>
-  </si>
-  <si>
     <t>Add item</t>
   </si>
   <si>
-    <t>Thêm món đồ</t>
-  </si>
-  <si>
     <t>Choose another photo</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>Delete item</t>
   </si>
   <si>
-    <t>Xóa món đồ</t>
-  </si>
-  <si>
     <t>Save</t>
   </si>
   <si>
@@ -102,15 +90,9 @@
     <t>Error analyzing item</t>
   </si>
   <si>
-    <t>Lỗi phân tích món đồ</t>
-  </si>
-  <si>
     <t>Pre-filling item information. You can edit later.</t>
   </si>
   <si>
-    <t>Đang nhập sẵn thông tin của món đồ. Bạn có thể chỉnh sửa sau khi quá trình này kết thúc.</t>
-  </si>
-  <si>
     <t>batch_add_item_screen.dart</t>
   </si>
   <si>
@@ -276,9 +258,6 @@
     <t>Trang phục cố định</t>
   </si>
   <si>
-    <t>Các món đồ trong trang phục này luôn được mặc cùng nhau. Mỗi món đồ chỉ được thuộc một trang phục cố định</t>
-  </si>
-  <si>
     <t>Items in this outfit are always worn together. Each item can only belong to one fixed outfit.</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>Cleaning closet…</t>
   </si>
   <si>
-    <t>Đang lau chùi tủ đồ</t>
-  </si>
-  <si>
     <t>splash_screen.dart</t>
   </si>
   <si>
@@ -352,6 +328,123 @@
   </si>
   <si>
     <t>Tên tủ đồ</t>
+  </si>
+  <si>
+    <t>Tủ đồ của bạn</t>
+  </si>
+  <si>
+    <t>Your closet</t>
+  </si>
+  <si>
+    <t>Tất cả vật phẩm</t>
+  </si>
+  <si>
+    <t>All items</t>
+  </si>
+  <si>
+    <t>By Closet</t>
+  </si>
+  <si>
+    <t>Theo tủ đồ</t>
+  </si>
+  <si>
+    <t>Add new closet</t>
+  </si>
+  <si>
+    <t>Thêm tủ đồ mới</t>
+  </si>
+  <si>
+    <t>home_page.dart</t>
+  </si>
+  <si>
+    <t>Gợi ý trang phục</t>
+  </si>
+  <si>
+    <t>Outfit suggestions</t>
+  </si>
+  <si>
+    <t>Xin chào,</t>
+  </si>
+  <si>
+    <t>Hello,</t>
+  </si>
+  <si>
+    <t>Outfit studio</t>
+  </si>
+  <si>
+    <t>Không gian sáng tạo</t>
+  </si>
+  <si>
+    <t>Tạo trang phục mới</t>
+  </si>
+  <si>
+    <t>Saved outfits</t>
+  </si>
+  <si>
+    <t>Create new outfit</t>
+  </si>
+  <si>
+    <t>Trang phục đã tạo</t>
+  </si>
+  <si>
+    <t>Xem tất cả</t>
+  </si>
+  <si>
+    <t>Đồ vật mới nhất</t>
+  </si>
+  <si>
+    <t>Lỗi phân tích đồ vật</t>
+  </si>
+  <si>
+    <t>Đang nhập sẵn thông tin. Bạn có thể chỉnh sửa sau khi quá trình này kết thúc.</t>
+  </si>
+  <si>
+    <t>Sửa đồ vật</t>
+  </si>
+  <si>
+    <t>Thêm đồ vật</t>
+  </si>
+  <si>
+    <t>Xóa đồ vật</t>
+  </si>
+  <si>
+    <t>Các đồ vật trong trang phục này luôn được mặc cùng nhau. Mỗi đồ vật chỉ được thuộc một trang phục cố định</t>
+  </si>
+  <si>
+    <t>Bạn có chắc chắn muốn xóa vĩnh viễn “…” không?</t>
+  </si>
+  <si>
+    <t>Đang lau dọn tủ đồ</t>
+  </si>
+  <si>
+    <t>Latest items</t>
+  </si>
+  <si>
+    <t>View all</t>
+  </si>
+  <si>
+    <t>Không có dữ liệu thời tiết.</t>
+  </si>
+  <si>
+    <t>Weather data unavailable.</t>
+  </si>
+  <si>
+    <t>Get suggestions</t>
+  </si>
+  <si>
+    <t>Nhận gợi ý</t>
+  </si>
+  <si>
+    <t>Bấm "Nhận gợi ý" để xem đề xuất trang phục!</t>
+  </si>
+  <si>
+    <t>Tap "Get Suggestions" to see outfit recommendations!</t>
+  </si>
+  <si>
+    <t>Cập nhật lúc</t>
+  </si>
+  <si>
+    <t>Last updated</t>
   </si>
 </sst>
 </file>
@@ -394,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -417,11 +510,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -430,6 +534,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,63 +871,63 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -828,24 +935,24 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -853,417 +960,536 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>43</v>
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>42</v>
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>45</v>
+      <c r="A30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>47</v>
+      <c r="A33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>49</v>
+      <c r="A35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>52</v>
+      <c r="A36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>54</v>
+      <c r="A37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>76</v>
+      <c r="A48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>82</v>
+      <c r="A54" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B57" s="3"/>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>86</v>
+      <c r="A58" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>88</v>
+      <c r="A60" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>43</v>
+      <c r="A62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>92</v>
+      <c r="A63" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>95</v>
+      <c r="A67" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>100</v>
+      <c r="A70" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>108</v>
+      <c r="A75" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>22</v>
+      <c r="A77" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A83:B83"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A57:B57"/>

</xml_diff>

<commit_message>
Dich outfits_hub_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD5D560-65D6-4266-AE4F-FA776DFEC773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B3F252-ED37-481F-8924-08B0A0E96271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="160">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Saved outfits</t>
   </si>
   <si>
-    <t>Create new outfit</t>
-  </si>
-  <si>
     <t>Trang phục đã tạo</t>
   </si>
   <si>
@@ -496,6 +493,18 @@
   </si>
   <si>
     <t>Stickers sẽ sớm được thêm vào.</t>
+  </si>
+  <si>
+    <t>outfits_hub_page.dart</t>
+  </si>
+  <si>
+    <t>Trang phục của bạn</t>
+  </si>
+  <si>
+    <t>Your outfits</t>
+  </si>
+  <si>
+    <t>Create a new outfit</t>
   </si>
 </sst>
 </file>
@@ -565,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -573,19 +582,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,19 +872,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -909,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -933,7 +939,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -941,7 +947,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -957,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -972,17 +978,17 @@
       <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -990,17 +996,17 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1015,7 +1021,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1043,10 +1049,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1065,40 +1071,40 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1111,26 +1117,26 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1199,16 +1205,16 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1221,32 +1227,32 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="3" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1255,20 +1261,20 @@
         <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1281,10 +1287,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1297,26 +1303,26 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="3"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -1327,24 +1333,24 @@
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>129</v>
+      <c r="B67" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="3"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1357,14 +1363,14 @@
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="3"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -1375,10 +1381,10 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1391,50 +1397,50 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B83" s="3"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
@@ -1445,10 +1451,10 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1461,112 +1467,112 @@
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B88" s="4" t="s">
+    </row>
+    <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    </row>
+    <row r="92" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+      <c r="B92" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B92" s="4" t="s">
+    </row>
+    <row r="93" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+    <row r="94" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+    </row>
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="B96" s="6"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
+      <c r="B98" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B98" s="4" t="s">
+    </row>
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1574,48 +1580,48 @@
       <c r="A102" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>127</v>
+      <c r="B102" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+    <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="B107" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1627,19 +1633,55 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="4" t="s">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
+      <c r="B112" s="6"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A96:B96"/>
@@ -1648,11 +1690,6 @@
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Dich profile_page.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B3F252-ED37-481F-8924-08B0A0E96271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D07AA6-720D-41C7-800F-E7AA43B4B9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Create a new outfit</t>
+  </si>
+  <si>
+    <t>profile_page.dart</t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,9 +1677,44 @@
         <v>116</v>
       </c>
     </row>
+    <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B117" s="6"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A117:B117"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>

</xml_diff>

<commit_message>
Dich get_outfit_suggestion_use_case.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D07AA6-720D-41C7-800F-E7AA43B4B9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECC8AD-8C1C-4B41-A5AC-EC570A7B9033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Screen" sheetId="1" r:id="rId1"/>
+    <sheet name="Domain" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="199">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -508,6 +509,120 @@
   </si>
   <si>
     <t>profile_page.dart</t>
+  </si>
+  <si>
+    <t>Chưa có tên</t>
+  </si>
+  <si>
+    <t>Unnamed</t>
+  </si>
+  <si>
+    <t>Trang cá nhân</t>
+  </si>
+  <si>
+    <t>Tải lại trang</t>
+  </si>
+  <si>
+    <t>Refresh page</t>
+  </si>
+  <si>
+    <t>Danh mục</t>
+  </si>
+  <si>
+    <t>Màu sắc</t>
+  </si>
+  <si>
+    <t>Mùa</t>
+  </si>
+  <si>
+    <t>Mục đích</t>
+  </si>
+  <si>
+    <t>Occasion</t>
+  </si>
+  <si>
+    <t>Tổng quan Tủ đồ</t>
+  </si>
+  <si>
+    <t>Closets overview</t>
+  </si>
+  <si>
+    <t>Thống kê</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Chưa có dữ liệu để thống kê.</t>
+  </si>
+  <si>
+    <t>No data for statistics</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>get_outfit_suggestion_use_case.dart</t>
+  </si>
+  <si>
+    <t>Lấy thời tiết theo tọa độ đã lưu:</t>
+  </si>
+  <si>
+    <t>Get weather by saved coordinates:</t>
+  </si>
+  <si>
+    <t>Dữ liệu vị trí thủ công bị thiếu, quay về mặc định.</t>
+  </si>
+  <si>
+    <t>Manual location data missing, reverting to default.</t>
+  </si>
+  <si>
+    <t>Getting weather by auto-detecting location…</t>
+  </si>
+  <si>
+    <t>Lấy thời tiết theo vị trí tự động…</t>
+  </si>
+  <si>
+    <t>Dịch vụ vị trí đang tắt, quay về mặc định.</t>
+  </si>
+  <si>
+    <t>Không có quyền truy cập vị trí, quay về mặc định.</t>
+  </si>
+  <si>
+    <t>Location services are disabled.</t>
+  </si>
+  <si>
+    <t>Location services are disabled, reverting to default.</t>
+  </si>
+  <si>
+    <t>Dịch vụ vị trí đang tắt.</t>
+  </si>
+  <si>
+    <t>Location permission are denied, reverting to default.</t>
+  </si>
+  <si>
+    <t>Location permission are denied.</t>
+  </si>
+  <si>
+    <t>Không có quyền truy cập vị trí.</t>
+  </si>
+  <si>
+    <t>Failed to load weather for suggestions, using default.</t>
+  </si>
+  <si>
+    <t>Lỗi khi lấy dữ liệu thời tiết cho gợi ý, sử dụng mặc định.</t>
+  </si>
+  <si>
+    <t>Please add items to your closet to get suggestions.</t>
+  </si>
+  <si>
+    <t>Vui lòng thêm đồ vào tủ để nhận gợi ý.</t>
   </si>
 </sst>
 </file>
@@ -875,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B124"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,32 +1799,120 @@
       <c r="B117" s="6"/>
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+      <c r="A120" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1732,4 +1935,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710F6A2B-9418-4F1B-9512-4519B03BD3D4}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dich save_outfit_use_case.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECC8AD-8C1C-4B41-A5AC-EC570A7B9033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E37D267-EB02-491E-B5D6-F5A81364CF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="206">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -623,6 +623,27 @@
   </si>
   <si>
     <t>Vui lòng thêm đồ vào tủ để nhận gợi ý.</t>
+  </si>
+  <si>
+    <t>save_outfit_use_case.dart</t>
+  </si>
+  <si>
+    <t>Đã lưu ảnh trang phục thành công tại:</t>
+  </si>
+  <si>
+    <t>Successfully saved outfit photo at:</t>
+  </si>
+  <si>
+    <t>File write error when saving outfit</t>
+  </si>
+  <si>
+    <t>Lỗi ghi file khi lưu trang phục</t>
+  </si>
+  <si>
+    <t>Không thể lưu ảnh của trang phục. Vui lòng thử lại.</t>
+  </si>
+  <si>
+    <t>Could not save outfit photo. Please try again.</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710F6A2B-9418-4F1B-9512-4519B03BD3D4}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,21 +2050,52 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dich validate_item_name_use_case.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E37D267-EB02-491E-B5D6-F5A81364CF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE40AC3C-7B37-46BC-81C4-619BBB3C0CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="211">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -644,6 +644,21 @@
   </si>
   <si>
     <t>Could not save outfit photo. Please try again.</t>
+  </si>
+  <si>
+    <t>validate_item_name_use_case.dart</t>
+  </si>
+  <si>
+    <t>... đã được sử dụng. Bạn vui lòng nhập tên khác. Có thể thêm số vào sau tên đồ vật (ví dụ: Áo 1, Áo 2,... để phân biệt).</t>
+  </si>
+  <si>
+    <t>… is already taken. Please use a different name. You can add numbers to distinguish items (e.g., Shirt 1, Shirt 2...).</t>
+  </si>
+  <si>
+    <t>Tên… của món đồ... đã trùng với món đồ … . Bạn vui lòng nhập tên khác. Có thể thêm số vào sau tên (ví dụ: Áo 1, Áo 2,... để dễ phân biệt).</t>
+  </si>
+  <si>
+    <t>... for item ...  is already used by item .... Please use a different name. You can add numbers to distinguish items (e.g., Shirt 1, Shirt 2...).</t>
   </si>
 </sst>
 </file>
@@ -1960,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710F6A2B-9418-4F1B-9512-4519B03BD3D4}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,22 +2095,49 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A17" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dich validate_required_fields_use_case.dart sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE40AC3C-7B37-46BC-81C4-619BBB3C0CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207AB251-7351-4FA5-BE4B-2FDD905F9B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="223">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -659,6 +659,42 @@
   </si>
   <si>
     <t>... for item ...  is already used by item .... Please use a different name. You can add numbers to distinguish items (e.g., Shirt 1, Shirt 2...).</t>
+  </si>
+  <si>
+    <t>… của món đồ ... đã được sử dụng. Bạn vui lòng nhập tên khác. Có thể thêm số vào sau tên đồ vật (ví dụ: Áo 1, Áo 2,... để phân biệt).</t>
+  </si>
+  <si>
+    <t>validate_required_fields_use_case.dart</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập tên đồ vật</t>
+  </si>
+  <si>
+    <t>Please enter item name</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn tủ đồ</t>
+  </si>
+  <si>
+    <t>Please select a closet</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn danh mục</t>
+  </si>
+  <si>
+    <t>Please select a category</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập tên cho đồ vật số</t>
+  </si>
+  <si>
+    <t>Please enter a name for Item</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn tủ quần áo cho đồ vật số</t>
+  </si>
+  <si>
+    <t>Please select a closet for Item</t>
   </si>
 </sst>
 </file>
@@ -1975,10 +2011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710F6A2B-9418-4F1B-9512-4519B03BD3D4}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,27 +2153,74 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+    <row r="20" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dich tat ca file notifiers sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,25 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207AB251-7351-4FA5-BE4B-2FDD905F9B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F24267-B407-452F-9CC7-A52B449FDE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen" sheetId="1" r:id="rId1"/>
     <sheet name="Domain" sheetId="2" r:id="rId2"/>
+    <sheet name="Notifiers" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="298">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -695,6 +707,231 @@
   </si>
   <si>
     <t>Please select a closet for Item</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn danh mục cho Món đồ số</t>
+  </si>
+  <si>
+    <t>Please select a category for Item</t>
+  </si>
+  <si>
+    <t>add_item_notifier.dart</t>
+  </si>
+  <si>
+    <t>Khác &gt; Khác</t>
+  </si>
+  <si>
+    <t>Other &gt; Other</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Vui lòng thêm ảnh cho món đồ.</t>
+  </si>
+  <si>
+    <t>Please add a photo for the item.</t>
+  </si>
+  <si>
+    <t>Lỗi khi lưu:</t>
+  </si>
+  <si>
+    <t>Save error:</t>
+  </si>
+  <si>
+    <t>Lỗi khi xóa:</t>
+  </si>
+  <si>
+    <t>Delete error:</t>
+  </si>
+  <si>
+    <t>batch_add_item_notifier.dart</t>
+  </si>
+  <si>
+    <t>city_selection_notifier.dart</t>
+  </si>
+  <si>
+    <t>Lỗi tìm kiếm địa điểm</t>
+  </si>
+  <si>
+    <t>Failed to search location</t>
+  </si>
+  <si>
+    <t>Lỗi tìm kiếm</t>
+  </si>
+  <si>
+    <t>Failed to search</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn một địa điểm từ danh sách gợi ý</t>
+  </si>
+  <si>
+    <t>Please select a location from the suggestions</t>
+  </si>
+  <si>
+    <t>Lỗi khi lưu cài đặt địa điểm</t>
+  </si>
+  <si>
+    <t>Failed to save location settings</t>
+  </si>
+  <si>
+    <t>closet_detail_notifier.dart</t>
+  </si>
+  <si>
+    <t>home_page_notifier.dart</t>
+  </si>
+  <si>
+    <t>Lỗi khi lấy gợi ý mới</t>
+  </si>
+  <si>
+    <t>Failed to get new suggestions</t>
+  </si>
+  <si>
+    <t>Không thể nhận gợi ý. Vui lòng thử lại.</t>
+  </si>
+  <si>
+    <t>Failed to get suggestions. Please try again.</t>
+  </si>
+  <si>
+    <t>item_filter_notifier.dart</t>
+  </si>
+  <si>
+    <t>Lỗi khi tải tất cả đồ vật</t>
+  </si>
+  <si>
+    <t>Failed to load all items</t>
+  </si>
+  <si>
+    <t>Lỗi tải vật phẩm</t>
+  </si>
+  <si>
+    <t>Failed to load item</t>
+  </si>
+  <si>
+    <t>outfit_builder_notifier.dart</t>
+  </si>
+  <si>
+    <t>Could not load items for sticker drawer.</t>
+  </si>
+  <si>
+    <t>Không thể tải đồ vật cho bộ tạo sticker</t>
+  </si>
+  <si>
+    <t>Vui lòng thêm ít nhất một đồ vật để lưu trang phục!</t>
+  </si>
+  <si>
+    <t>Please add at least one item to save the outfit!</t>
+  </si>
+  <si>
+    <t>Lỗi:... Một đồ vật đã thuộc một Trang phục cố định khác.</t>
+  </si>
+  <si>
+    <t>Error:... An item already belongs to another fixed outfit.</t>
+  </si>
+  <si>
+    <t>Lỗi khi lưu trang phục:</t>
+  </si>
+  <si>
+    <t>outfit_detail_notifier.dart</t>
+  </si>
+  <si>
+    <t>Failed to save outfit:</t>
+  </si>
+  <si>
+    <t>Lỗi khi cập nhật tên trang phục</t>
+  </si>
+  <si>
+    <t>Failed to update outfit name</t>
+  </si>
+  <si>
+    <t>Một đồ vật</t>
+  </si>
+  <si>
+    <t>An item</t>
+  </si>
+  <si>
+    <t>Lỗi: ... đã thuộc một Trang phục cố định khác.</t>
+  </si>
+  <si>
+    <t>Error: ... already belongs to another fixed outfit.</t>
+  </si>
+  <si>
+    <t>Failed to update fixed outfit</t>
+  </si>
+  <si>
+    <t>Lỗi khi cập nhật Trang phục cố định</t>
+  </si>
+  <si>
+    <t>Đã có lỗi không xác định xảy ra.</t>
+  </si>
+  <si>
+    <t>Something went wrong.</t>
+  </si>
+  <si>
+    <t>Lỗi khi xóa trang phục</t>
+  </si>
+  <si>
+    <t>Failed to delete outfit</t>
+  </si>
+  <si>
+    <t>profile_page_notifier.dart</t>
+  </si>
+  <si>
+    <t>Bắt đầu tải dữ liệu Profile…</t>
+  </si>
+  <si>
+    <t>Loading profile data…</t>
+  </si>
+  <si>
+    <t>1. Tải SharedPreferences thành công.</t>
+  </si>
+  <si>
+    <t>1. SharedPreferences loaded successfully</t>
+  </si>
+  <si>
+    <t>2. Khởi tạo các Repositories thành công.</t>
+  </si>
+  <si>
+    <t>2. Repositories initialized successfully.</t>
+  </si>
+  <si>
+    <t>Người dùng MinCloset</t>
+  </si>
+  <si>
+    <t>MinCloset user</t>
+  </si>
+  <si>
+    <t>3. Đọc dữ liệu từ SharedPreferences thành công.</t>
+  </si>
+  <si>
+    <t>3. Successfully read SharedPreferences.</t>
+  </si>
+  <si>
+    <t>4. Tải tất cả Items từ CSDL thành công.</t>
+  </si>
+  <si>
+    <t>4. Successfully loaded all items from database.</t>
+  </si>
+  <si>
+    <t>5. Tải tất cả Closets từ CSDL thành công.</t>
+  </si>
+  <si>
+    <t>5. Successfully loaded all closets from database.</t>
+  </si>
+  <si>
+    <t>6. Tải tất cả Outfits từ CSDL thành công.</t>
+  </si>
+  <si>
+    <t>6. Successfully loaded all outfits from database.</t>
+  </si>
+  <si>
+    <t>7. Tính toán thống kê thành công.</t>
+  </si>
+  <si>
+    <t>Statistics calculated successfully.</t>
   </si>
 </sst>
 </file>
@@ -737,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -760,11 +997,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -780,6 +1028,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1064,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710F6A2B-9418-4F1B-9512-4519B03BD3D4}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,8 +2459,12 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -2224,4 +2479,376 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28D71B4-9B11-4D69-A483-A516CB616912}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="2" max="2" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dich tat ca file widgets sang tieng Anh
</commit_message>
<xml_diff>
--- a/_UI Language.xlsx
+++ b/_UI Language.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F24267-B407-452F-9CC7-A52B449FDE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF5BF09-8D5A-4A35-98E3-6C83B7026DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen" sheetId="1" r:id="rId1"/>
     <sheet name="Domain" sheetId="2" r:id="rId2"/>
     <sheet name="Notifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="widgets" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="367">
   <si>
     <t>add_item_screen.dart</t>
   </si>
@@ -931,7 +932,214 @@
     <t>7. Tính toán thống kê thành công.</t>
   </si>
   <si>
-    <t>Statistics calculated successfully.</t>
+    <t>7. Statistics calculated successfully.</t>
+  </si>
+  <si>
+    <t>8. Cập nhật state thành công! Hoàn tất tải trang Profile.</t>
+  </si>
+  <si>
+    <t>8. State updated successfully! Profile page loading complete.</t>
+  </si>
+  <si>
+    <t>Lỗi khi tải dữ liệu trang cá nhân</t>
+  </si>
+  <si>
+    <t>Failed to load profile data.</t>
+  </si>
+  <si>
+    <t>Không thể tải dữ liệu. Vui lòng thử lại.</t>
+  </si>
+  <si>
+    <t>Failed to load data. Please try again.</t>
+  </si>
+  <si>
+    <t>category_selector.dart</t>
+  </si>
+  <si>
+    <t>Danh mục *</t>
+  </si>
+  <si>
+    <t>Category *</t>
+  </si>
+  <si>
+    <t>Chưa chọn</t>
+  </si>
+  <si>
+    <t>None selected</t>
+  </si>
+  <si>
+    <t>filter_bottom_sheet.dart</t>
+  </si>
+  <si>
+    <t>Bộ lọc</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Closet</t>
+  </si>
+  <si>
+    <t>Tất cả tủ đồ</t>
+  </si>
+  <si>
+    <t>All closets</t>
+  </si>
+  <si>
+    <t>Tất cả danh mục</t>
+  </si>
+  <si>
+    <t>All categories</t>
+  </si>
+  <si>
+    <t>Chất liệu</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Họa tiết</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Xóa bộ lọc</t>
+  </si>
+  <si>
+    <t>Clear filters</t>
+  </si>
+  <si>
+    <t>Áp dụng</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>global_add_button.dart</t>
+  </si>
+  <si>
+    <t>Đã chọn tối đa 10 ảnh. Các ảnh thừa đã được bỏ qua.</t>
+  </si>
+  <si>
+    <t>Maximum of 10 photos selected. Extra photos were skipped.</t>
+  </si>
+  <si>
+    <t>Chọn từ Thư viện ảnh (tối đa 10 một lượt)</t>
+  </si>
+  <si>
+    <t>Choose from album (up to 10)</t>
+  </si>
+  <si>
+    <t>item_browser_view.dart</t>
+  </si>
+  <si>
+    <t>Không tìm thấy đồ vật nào.</t>
+  </si>
+  <si>
+    <t>No items available.</t>
+  </si>
+  <si>
+    <t>Tủ đồ của bạn chưa có đồ vật nào.</t>
+  </si>
+  <si>
+    <t>Your closet is empty</t>
+  </si>
+  <si>
+    <t>item_detail_form.dart</t>
+  </si>
+  <si>
+    <t>Tên món đồ *</t>
+  </si>
+  <si>
+    <t>Chọn tủ đồ *</t>
+  </si>
+  <si>
+    <t>Item name *</t>
+  </si>
+  <si>
+    <t>Select closet *</t>
+  </si>
+  <si>
+    <t>Lỗi tải tủ đồ:</t>
+  </si>
+  <si>
+    <t>Failed to load closet:</t>
+  </si>
+  <si>
+    <t>item_search_filter_bar.dart</t>
+  </si>
+  <si>
+    <t>Tìm kiếm vật phẩm…</t>
+  </si>
+  <si>
+    <t>Search items…</t>
+  </si>
+  <si>
+    <t>multi_select_chip_field.dart</t>
+  </si>
+  <si>
+    <t>Chưa có</t>
+  </si>
+  <si>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>outfit_actions_menu.dart</t>
+  </si>
+  <si>
+    <t>Sửa tên</t>
+  </si>
+  <si>
+    <t>Chia sẻ</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Đổi tên trang phục</t>
+  </si>
+  <si>
+    <t>Rename</t>
+  </si>
+  <si>
+    <t>Rename outfit</t>
+  </si>
+  <si>
+    <t>Tên mới</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>Cùng xem trang phục của tôi nhé!</t>
+  </si>
+  <si>
+    <t>Let check out my outfit:</t>
+  </si>
+  <si>
+    <t>Permanently delete outfit</t>
+  </si>
+  <si>
+    <t>Xóa vĩnh viễn trang phục</t>
+  </si>
+  <si>
+    <t>Deleted outfit</t>
+  </si>
+  <si>
+    <t>Đã xóa trang phục</t>
+  </si>
+  <si>
+    <t>stats_overview_card.dart</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Outfit</t>
+  </si>
+  <si>
+    <t>Đồ vật</t>
   </si>
 </sst>
 </file>
@@ -1001,18 +1209,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1028,6 +1238,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1315,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,15 +2696,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28D71B4-9B11-4D69-A483-A516CB616912}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2814,27 +3027,51 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="1" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="1" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="1" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2851,4 +3088,440 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625FE846-4142-4EEE-8BE7-286010C2D5AA}">
+  <dimension ref="A1:B61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="B58" s="6"/>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A38:B38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>